<commit_message>
Fix stepper import tax type
</commit_message>
<xml_diff>
--- a/public/templates/Plantilla Bulk Import.xlsx
+++ b/public/templates/Plantilla Bulk Import.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>sku</t>
   </si>
@@ -26,6 +26,9 @@
     <t>is_service</t>
   </si>
   <si>
+    <t>tax_type</t>
+  </si>
+  <si>
     <t>P001</t>
   </si>
   <si>
@@ -50,12 +53,18 @@
     <t>Mouse Inalámbrico Logitech</t>
   </si>
   <si>
+    <t>Exento</t>
+  </si>
+  <si>
     <t>P005</t>
   </si>
   <si>
     <t>Disco Duro Externo 1TB</t>
   </si>
   <si>
+    <t>Exonerado</t>
+  </si>
+  <si>
     <t>P006</t>
   </si>
   <si>
@@ -68,10 +77,16 @@
     <t>Instalación de Software</t>
   </si>
   <si>
+    <t>GRAVADO_15</t>
+  </si>
+  <si>
     <t>P008</t>
   </si>
   <si>
     <t>Impresora Multifuncional</t>
+  </si>
+  <si>
+    <t>GRAVADO_18</t>
   </si>
   <si>
     <t>P009</t>
@@ -186,11 +201,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="9" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -431,68 +449,86 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>15000.0</v>
       </c>
+      <c r="E2" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>3500.0</v>
       </c>
+      <c r="E3" s="2">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>850.0</v>
       </c>
+      <c r="E4" s="2">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>450.0</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1">
         <v>1200.0</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1">
         <v>500.0</v>
@@ -500,13 +536,16 @@
       <c r="D7" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="E7" s="2">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1">
         <v>350.0</v>
@@ -514,24 +553,30 @@
       <c r="D8" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1">
         <v>2800.0</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1">
         <v>750.0</v>
@@ -539,13 +584,16 @@
       <c r="D10" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="E10" s="2">
+        <v>0.18</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1">
         <v>950.0</v>
@@ -573,123 +621,123 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1">
         <v>8.019995123456E12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1">
         <v>5.019988765432E12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1">
         <v>1.019977654321E12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1">
         <v>8.01996654321E12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B6" s="1">
         <v>5.019955432109E12</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1">
         <v>1.019944321098E12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1">
         <v>8.019933210987E12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1">
         <v>5.019922109876E12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1">
         <v>1.019911098765E12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1">
         <v>8.019900987654E12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>